<commit_message>
Impemented a miniturized version mainly focussing on pre-filtration
</commit_message>
<xml_diff>
--- a/hardware/BOM/External hardware components.xlsx
+++ b/hardware/BOM/External hardware components.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" tabRatio="477"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8010" windowHeight="7800" tabRatio="477" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="EXTERNAL COMPONENTS" sheetId="4" r:id="rId1"/>
+    <sheet name="(Large) EXTERNAL COMPONENTS" sheetId="4" r:id="rId1"/>
+    <sheet name="(MINI) EXTERNAL COMPONENTS" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="123">
   <si>
     <t>Component</t>
   </si>
@@ -337,6 +338,57 @@
   </si>
   <si>
     <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Hollow UF membrane</t>
+  </si>
+  <si>
+    <t>A lightweight, palm-sized Sawyer Mini water filtration kit that includes a reusable pouch, syringe, and straw, offering high-performance 0.1-micron filtration to remove bacteria, protozoa, and microplastics, with versatile compatibility for outdoor use, travel, and emergency preparedness.</t>
+  </si>
+  <si>
+    <t>Sawyer</t>
+  </si>
+  <si>
+    <t>sawyer.com [https://www.sawyer.com/product/mini-water-filtration-system-blue#product-details]</t>
+  </si>
+  <si>
+    <t>Carbon filter</t>
+  </si>
+  <si>
+    <t>A Ronaqua T33 inline coconut-shell activated carbon filter designed for reverse osmosis systems and similar applications, used as a pre/post polishing stage to improve water taste and odor, NSF-certified, easy to install, and typically replaced every two years.</t>
+  </si>
+  <si>
+    <t>Ronaqua</t>
+  </si>
+  <si>
+    <t>‎FBA_RA-T33</t>
+  </si>
+  <si>
+    <t>amazon.com [https://www.amazon.com/Inline-Coconut-Activated-Membrane-Reduction/dp/B0719SHH9X?th=1]</t>
+  </si>
+  <si>
+    <t>Turbidity sensor</t>
+  </si>
+  <si>
+    <t>Micro Pressure sensor</t>
+  </si>
+  <si>
+    <t>Search: "Pressure Transducer Sensor 5V 80psi".</t>
+  </si>
+  <si>
+    <t>Flow sensor</t>
+  </si>
+  <si>
+    <t>buy the small one</t>
+  </si>
+  <si>
+    <t>YF-S401</t>
+  </si>
+  <si>
+    <t>Micro Diaphragm pump</t>
+  </si>
+  <si>
+    <t>Mechanical check valve</t>
   </si>
 </sst>
 </file>
@@ -684,9 +736,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1246,4 +1298,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="25.90625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="12.90625" customWidth="1"/>
+    <col min="5" max="5" width="13.81640625" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" customWidth="1"/>
+    <col min="8" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="13.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="1" customFormat="1" ht="38.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3">
+        <v>28.99</v>
+      </c>
+      <c r="H3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
+      <c r="D4" t="s">
+        <v>112</v>
+      </c>
+      <c r="E4" t="s">
+        <v>113</v>
+      </c>
+      <c r="G4">
+        <v>12.49</v>
+      </c>
+      <c r="H4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C8" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E9" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>